<commit_message>
QA manual CoderHouse 2025
</commit_message>
<xml_diff>
--- a/Testing Coca-Cola y Chicos.Net/Celfar/Carolina Pena - Defectos-CasosPrueba-Celfar V1.xlsx
+++ b/Testing Coca-Cola y Chicos.Net/Celfar/Carolina Pena - Defectos-CasosPrueba-Celfar V1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\unpaz caro\curso testing\Celfar\Evidencias defectos-V1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carop\OneDrive\Escritorio\carpeta caro\portfolio testing\Testing Coca-Cola y Chicos.Net\Celfar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE69BC5-B7EE-4E85-A10A-60A07EF66DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DACFA32-93A5-4A19-8F41-7C11101F24EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{34B9A7D9-D416-47A8-9F25-6D92BC06F586}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{34B9A7D9-D416-47A8-9F25-6D92BC06F586}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de prueba" sheetId="1" r:id="rId1"/>
@@ -1874,12 +1874,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1892,9 +1952,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1903,63 +1960,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3262,22 +3262,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588DA04C-C167-4902-AF5A-D869F34C19A2}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G22" workbookViewId="0">
+    <sheetView topLeftCell="G22" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="91.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="126" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="74.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="119.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="74.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="119.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3287,7 +3287,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3297,14 +3297,14 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>38</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>21</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
         <v>20</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="34"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -3462,7 +3462,7 @@
       <c r="H9" s="35"/>
       <c r="I9" s="34"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="34"/>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
@@ -3475,7 +3475,7 @@
       <c r="H10" s="35"/>
       <c r="I10" s="34"/>
     </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>23</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>24</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>25</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>26</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>27</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>28</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>51</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>52</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>53</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>54</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>58</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>61</v>
       </c>
@@ -3852,10 +3852,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F26" s="23"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F27" s="23"/>
     </row>
   </sheetData>
@@ -3879,40 +3879,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E14B773-298B-4631-BC81-D8D28750EAF2}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:C35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="102.44140625" customWidth="1"/>
+    <col min="2" max="2" width="43.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.140625" customWidth="1"/>
-    <col min="7" max="7" width="47.28515625" customWidth="1"/>
-    <col min="8" max="8" width="62.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.109375" customWidth="1"/>
+    <col min="7" max="7" width="47.33203125" customWidth="1"/>
+    <col min="8" max="8" width="62.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="57"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="54"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16"/>
       <c r="H2" s="17"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
@@ -3941,8 +3941,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="42" t="s">
         <v>78</v>
       </c>
       <c r="B4" s="44" t="s">
@@ -3954,99 +3954,99 @@
       <c r="D4" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="G4" s="48" t="s">
+      <c r="G4" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="62"/>
-      <c r="I4" s="60" t="s">
+      <c r="H4" s="39"/>
+      <c r="I4" s="38" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="63"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="43"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="40"/>
       <c r="I5" s="34"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="63"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="43"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="40"/>
       <c r="I6" s="34"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="63"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="43"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="40"/>
       <c r="I7" s="34"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="63"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="43"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="40"/>
       <c r="I8" s="34"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="63"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="43"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="40"/>
       <c r="I9" s="34"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="63"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="43"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="40"/>
       <c r="I10" s="34"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="59"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="64"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="49"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="41"/>
       <c r="I11" s="34"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="42" t="s">
         <v>72</v>
       </c>
       <c r="B12" s="44" t="s">
@@ -4061,76 +4061,76 @@
       <c r="E12" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="48" t="s">
+      <c r="F12" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="G12" s="48" t="s">
+      <c r="G12" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="H12" s="62"/>
+      <c r="H12" s="39"/>
       <c r="I12" s="34" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="43"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
       <c r="E13" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="63"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="40"/>
       <c r="I13" s="34"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="63"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="43"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="40"/>
       <c r="I14" s="34"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="63"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="43"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="40"/>
       <c r="I15" s="34"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="63"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="43"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="40"/>
       <c r="I16" s="34"/>
     </row>
-    <row r="17" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="59"/>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="64"/>
+    <row r="17" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="49"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="41"/>
       <c r="I17" s="34"/>
     </row>
-    <row r="18" spans="1:9" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+    <row r="18" spans="1:9" ht="113.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="42" t="s">
         <v>86</v>
       </c>
       <c r="B18" s="44" t="s">
@@ -4145,10 +4145,10 @@
       <c r="E18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="48" t="s">
+      <c r="F18" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G18" s="48" t="s">
+      <c r="G18" s="46" t="s">
         <v>90</v>
       </c>
       <c r="H18" s="19" t="s">
@@ -4158,38 +4158,38 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
+    <row r="19" spans="1:9" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="43"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
       <c r="E19" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
       <c r="H19" s="19" t="s">
         <v>92</v>
       </c>
       <c r="I19" s="34"/>
     </row>
-    <row r="20" spans="1:9" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
+    <row r="20" spans="1:9" ht="117.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="43"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
       <c r="E20" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
       <c r="H20" s="19" t="s">
         <v>93</v>
       </c>
       <c r="I20" s="34"/>
     </row>
-    <row r="21" spans="1:9" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="58" t="s">
+    <row r="21" spans="1:9" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="42" t="s">
         <v>94</v>
       </c>
       <c r="B21" s="44" t="s">
@@ -4204,10 +4204,10 @@
       <c r="E21" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="48" t="s">
+      <c r="F21" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="G21" s="48" t="s">
+      <c r="G21" s="46" t="s">
         <v>100</v>
       </c>
       <c r="H21" s="20" t="s">
@@ -4217,38 +4217,38 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
+    <row r="22" spans="1:9" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="43"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
       <c r="E22" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
       <c r="H22" s="21" t="s">
         <v>105</v>
       </c>
       <c r="I22" s="34"/>
     </row>
-    <row r="23" spans="1:9" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
+    <row r="23" spans="1:9" ht="107.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="43"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
       <c r="H23" s="21" t="s">
         <v>93</v>
       </c>
       <c r="I23" s="34"/>
     </row>
-    <row r="24" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="58" t="s">
+    <row r="24" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="42" t="s">
         <v>99</v>
       </c>
       <c r="B24" s="44" t="s">
@@ -4263,10 +4263,10 @@
       <c r="E24" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="48" t="s">
+      <c r="F24" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="G24" s="48" t="s">
+      <c r="G24" s="46" t="s">
         <v>104</v>
       </c>
       <c r="H24" s="20" t="s">
@@ -4276,38 +4276,38 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
+    <row r="25" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="43"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
       <c r="E25" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
       <c r="H25" s="21" t="s">
         <v>92</v>
       </c>
       <c r="I25" s="34"/>
     </row>
-    <row r="26" spans="1:9" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
+    <row r="26" spans="1:9" ht="109.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="43"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
       <c r="E26" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
       <c r="H26" s="21" t="s">
         <v>93</v>
       </c>
       <c r="I26" s="34"/>
     </row>
-    <row r="27" spans="1:9" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="58" t="s">
+    <row r="27" spans="1:9" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="42" t="s">
         <v>106</v>
       </c>
       <c r="B27" s="44" t="s">
@@ -4319,13 +4319,13 @@
       <c r="D27" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="F27" s="48" t="s">
+      <c r="F27" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="G27" s="48" t="s">
+      <c r="G27" s="46" t="s">
         <v>90</v>
       </c>
       <c r="H27" s="14" t="s">
@@ -4335,34 +4335,34 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
+    <row r="28" spans="1:9" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="43"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
       <c r="H28" s="15" t="s">
         <v>105</v>
       </c>
       <c r="I28" s="34"/>
     </row>
-    <row r="29" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
+    <row r="29" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="43"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
       <c r="H29" s="15" t="s">
         <v>93</v>
       </c>
       <c r="I29" s="34"/>
     </row>
-    <row r="30" spans="1:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="58" t="s">
+    <row r="30" spans="1:9" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="42" t="s">
         <v>139</v>
       </c>
       <c r="B30" s="44" t="s">
@@ -4374,13 +4374,13 @@
       <c r="D30" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="48" t="s">
+      <c r="E30" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="F30" s="48" t="s">
+      <c r="F30" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="48" t="s">
+      <c r="G30" s="46" t="s">
         <v>104</v>
       </c>
       <c r="H30" s="14" t="s">
@@ -4390,94 +4390,132 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
+    <row r="31" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="43"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
       <c r="H31" s="15" t="s">
         <v>105</v>
       </c>
       <c r="I31" s="34"/>
     </row>
-    <row r="32" spans="1:9" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="50"/>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
+    <row r="32" spans="1:9" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="43"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
       <c r="H32" s="15" t="s">
         <v>93</v>
       </c>
       <c r="I32" s="44"/>
     </row>
-    <row r="33" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="49" t="s">
+    <row r="33" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="C33" s="52" t="s">
+      <c r="C33" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="52" t="s">
+      <c r="D33" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="38" t="s">
+      <c r="E33" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="F33" s="38" t="s">
+      <c r="F33" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="41" t="s">
+      <c r="G33" s="61" t="s">
         <v>146</v>
       </c>
       <c r="H33" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="I33" s="45" t="s">
+      <c r="I33" s="64" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="42"/>
+    <row r="34" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="43"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="62"/>
       <c r="H34" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="I34" s="46"/>
-    </row>
-    <row r="35" spans="1:9" ht="120.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="51"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="43"/>
+      <c r="I34" s="65"/>
+    </row>
+    <row r="35" spans="1:9" ht="120.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="56"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="63"/>
       <c r="H35" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="I35" s="47"/>
+      <c r="I35" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="I4:I11"/>
-    <mergeCell ref="I12:I17"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="G27:G29"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="G30:G32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="B4:B11"/>
+    <mergeCell ref="C4:C11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="F4:F11"/>
+    <mergeCell ref="G4:G11"/>
+    <mergeCell ref="H4:H11"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="D12:D17"/>
+    <mergeCell ref="F12:F17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="D21:D23"/>
     <mergeCell ref="H12:H17"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="B30:B32"/>
@@ -4494,49 +4532,11 @@
     <mergeCell ref="G21:G23"/>
     <mergeCell ref="G24:G26"/>
     <mergeCell ref="G12:G17"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="D12:D17"/>
-    <mergeCell ref="F12:F17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="B4:B11"/>
-    <mergeCell ref="C4:C11"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="F4:F11"/>
-    <mergeCell ref="G4:G11"/>
-    <mergeCell ref="H4:H11"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="I30:I32"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="G27:G29"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="G30:G32"/>
+    <mergeCell ref="I4:I11"/>
+    <mergeCell ref="I12:I17"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>